<commit_message>
Used "Number1" and "Number2" in all examples for non-maths professors and non-English natives.
Added comments to the feature files prior to the .xlsx references for added clarity.
</commit_message>
<xml_diff>
--- a/ExcelExample/ExcelExample/Features/CalculatorAdd.feature.xlsx
+++ b/ExcelExample/ExcelExample/Features/CalculatorAdd.feature.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17766"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Add two positive numbers" sheetId="1" r:id="rId1"/>
     <sheet name="Add two negative numbers" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,9 +28,6 @@
     <t>I have entered</t>
   </si>
   <si>
-    <t>&lt;SummandOne&gt;</t>
-  </si>
-  <si>
     <t>into the calculator</t>
   </si>
   <si>
@@ -40,9 +37,6 @@
     <t>I have also entered</t>
   </si>
   <si>
-    <t>&lt;SummandTwo&gt;</t>
-  </si>
-  <si>
     <t>When</t>
   </si>
   <si>
@@ -58,12 +52,6 @@
     <t>Examples:</t>
   </si>
   <si>
-    <t>SummandOne</t>
-  </si>
-  <si>
-    <t>SummandTwo</t>
-  </si>
-  <si>
     <t>Result</t>
   </si>
   <si>
@@ -71,12 +59,24 @@
   </si>
   <si>
     <t>The result should be</t>
+  </si>
+  <si>
+    <t>&lt;Number1&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Number2&gt;</t>
+  </si>
+  <si>
+    <t>Number1</t>
+  </si>
+  <si>
+    <t>Number2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -390,8 +390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -410,62 +410,62 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -525,8 +525,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,62 +544,62 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D7" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>